<commit_message>
updated similarity matches files
</commit_message>
<xml_diff>
--- a/hsim-experiment/harmonic_similarity_split/harmonic_similarity_matches_1.xlsx
+++ b/hsim-experiment/harmonic_similarity_split/harmonic_similarity_matches_1.xlsx
@@ -483,81 +483,85 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>isophonics_201</t>
+          <t>schubert-winterreise_61</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>isophonics_224</t>
+          <t>schubert-winterreise_89</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.1302083333333333</v>
+        <v>0.1177257525083612</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[['C:7', 'F:maj', 'Bb:maj']]</t>
+          <t>[['C:min/D#', 'G:min/D', 'D:7', 'G:min']]</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[['E:7', 'A', 'D']]</t>
+          <t>[['C:min/G', 'G:min', 'D:7', 'G:min']]</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[(63.251, 70.247)]</t>
+          <t>[(42.14, 44.36)]</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[(26.987959, 33.059977)]</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
+          <t>[(2.98, 6.7)]</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>spotify:track:68YORkKP9uvlOQFMZZZwH5</t>
+        </is>
+      </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>spotify:track:6dGnYIeXmHdcikdzNNDMm2</t>
+          <t>spotify:track:4lrfYSnZmpXdCWuWqVo8L0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>schubert-winterreise_177</t>
+          <t>schubert-winterreise_164</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>schubert-winterreise_82</t>
+          <t>schubert-winterreise_157</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.1036789297658863</v>
+        <v>0.2753623188405797</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[['A:min/E', 'E:7', 'A:min'], ['A:min', 'D:min/A', 'A:min']]</t>
+          <t>[['A:min', 'D:min', 'A:min', 'E:7', 'A:min']]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[['G:min', 'D:7', 'G:min'], ['G:min', 'C:min/G', 'G:min']]</t>
+          <t>[['F:min', 'A#:min/F', 'F:min', 'C:7', 'F:min']]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>[(83.1, 90.02), (28.14, 36.1)]</t>
+          <t>[(14.52, 29.1)]</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>[(3.1, 5.58), (0.5, 3.9)]</t>
+          <t>[(0.3, 4.8)]</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>spotify:track:2g41AZ58LFdQLxmWx82ujI</t>
+          <t>spotify:track:3OD2uwEUQKg0WyW9Lewata</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -569,35 +573,35 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>schubert-winterreise_21</t>
+          <t>isophonics_30</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>schubert-winterreise_200</t>
+          <t>isophonics_107</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.3028846153846154</v>
+        <v>0.1894736842105263</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[['D#:min', 'A#:maj', 'D#:min']]</t>
+          <t>[['A', 'A', 'D']]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[['E:min', 'B:maj', 'E:min']]</t>
+          <t>[['E', 'E', 'A']]</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>[(2.66, 7.98)]</t>
+          <t>[(14.448702, 17.908476)]</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>[(81.28, 89.42)]</t>
+          <t>[(122.976598, 130.383764)]</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
@@ -606,35 +610,35 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>schubert-winterreise_42</t>
+          <t>isophonics_297</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>schubert-winterreise_206</t>
+          <t>isophonics_199</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0.06725146198830409</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[['G:(3,5,b7,b9)', 'C:min', 'E:dim7'], ['G#:maj', 'D#:(3,5,b7,b9)', 'G#:maj'], ['F#:dim7', 'G:maj', 'C:min']]</t>
+          <t>[['C', 'D', 'G']]</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[['A:(3,5,b7,b9)', 'D:min', 'F#:dim7'], ['A#:maj', 'F:(3,5,b7,b9)', 'A#:maj'], ['G#:dim7', 'A:maj', 'D:min']]</t>
+          <t>[['G', 'A', 'D']]</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>[(11.76, 15.64), (20.54, 23.16), (16.24, 17.66)]</t>
+          <t>[(18.675377, 23.261318)]</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>[(12.98, 17.2), (22.6, 25.72), (17.9, 19.44)]</t>
+          <t>[(2.088054, 5.756807)]</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
@@ -643,117 +647,121 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>isophonics_140</t>
+          <t>schubert-winterreise_69</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>isophonics_283</t>
+          <t>schubert-winterreise_6</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.1384615384615385</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[['G', 'G', 'C']]</t>
+          <t>[['B:min', 'F#:7/A#', 'B:min']]</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>[['G', 'G', 'C']]</t>
+          <t>[['B:min/F#', 'F#:7', 'B:min']]</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>[(10.090897, 16.615704)]</t>
+          <t>[(42.36, 50.36)]</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>[(60.180884, 68.841927)]</t>
+          <t>[(79.42, 86.02)]</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>spotify:track:3VbGCXWRiouAq8VyMYN2MI</t>
+          <t>spotify:track:1yerCi2iQCVkdHG6rdRn7R</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>spotify:track:3tGhRLgcCP6SIZU3tbGl7l</t>
+          <t>spotify:track:2g41AZ58LFdQLxmWx82ujI</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>isophonics_234</t>
+          <t>isophonics_93</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>schubert-winterreise_145</t>
+          <t>isophonics_261</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.4666666666666667</v>
+        <v>0.1154891304347826</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[['Eb/5', 'Ab/2', 'Eb']]</t>
+          <t>[['C', 'F:maj6', 'C']]</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>[['D:maj/A', 'G:maj', 'D:maj/A']]</t>
+          <t>[['G', 'A:min7', 'G/3']]</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>[(75.439, 83.381)]</t>
+          <t>[(36.36882, 43.729546)]</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>[(143.58, 148.16)]</t>
+          <t>[(10.107052, 14.565283)]</t>
         </is>
       </c>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>spotify:track:2B4Y9u4ERAFiMo13XPJyGP</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>jaah_32</t>
+          <t>isophonics_31</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>isophonics_294</t>
+          <t>isophonics_251</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.06828087167070218</v>
+        <v>0.3101503759398496</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>[['G', 'G', 'G']]</t>
+          <t>[['E:min', 'C', 'G', 'C', 'G']]</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>[['G/3', 'G', 'G']]</t>
+          <t>[['B:min', 'G', 'D', 'G', 'D']]</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>[(3.01, 7.27)]</t>
+          <t>[(11.110106, 30.271443)]</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>[(1.366439, 5.255782)]</t>
+          <t>[(22.141972, 33.3456)]</t>
         </is>
       </c>
       <c r="H8" t="inlineStr"/>
@@ -762,35 +770,35 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>schubert-winterreise_159</t>
+          <t>isophonics_111</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>schubert-winterreise_204</t>
+          <t>schubert-winterreise_63</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>0.1613636363636363</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>[['E:(3,b5,b7)/G#', 'A:maj', 'E:(3,b5,b7)/A#', 'A:maj', 'E:(3,b5,b7)/A#', 'A:maj', 'E:(3,b5,b7)/A#', 'A:maj', 'E:(3,b5,b7)/A#', 'A:maj', 'E:(3,b5,b7)/A#']]</t>
+          <t>[['C', 'G:7', 'C']]</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>[['E:(3,b5,b7)/G#', 'A:maj', 'E:(3,b5,b7)/A#', 'A:maj', 'E:(3,b5,b7)/A#', 'A:maj', 'E:(3,b5,b7)/A#', 'A:maj', 'E:(3,b5,b7)/A#', 'A:maj', 'E:(3,b5,b7)/A#']]</t>
+          <t>[['C/G', 'G:7', 'C']]</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>[(47.34, 52.74)]</t>
+          <t>[(70.519024, 75.720294)]</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>[(43.1, 47.74)]</t>
+          <t>[(253.84, 257.6)]</t>
         </is>
       </c>
       <c r="H9" t="inlineStr"/>
@@ -799,12 +807,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>isophonics_164</t>
+          <t>schubert-winterreise_188</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>schubert-winterreise_108</t>
+          <t>isophonics_212</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -812,145 +820,141 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>[['C:min', 'F:min', 'C:min']]</t>
+          <t>[['F:maj', 'A#:maj', 'F:maj', 'A#:maj', 'F:maj']]</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>[['A:min', 'D:min', 'A:min']]</t>
+          <t>[['D', 'G', 'D', 'G', 'D']]</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>[(7.702, 13.841)]</t>
+          <t>[(128.76, 134.6)]</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>[(10.88, 16.76)]</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>spotify:track:3OD2uwEUQKg0WyW9Lewata</t>
-        </is>
-      </c>
+          <t>[(46.93228, 57.636679)]</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>spotify:track:1nvxQGWCnikMK7a4HYQvSx</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>schubert-winterreise_0</t>
+          <t>isophonics_213</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>schubert-winterreise_173</t>
+          <t>jaah_43</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.1036789297658863</v>
+        <v>0.1607142857142857</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>[['B:min/F#', 'F#:7', 'B:min'], ['B:min', 'E:min/B', 'B:min']]</t>
+          <t>[['E', 'E:7', 'A']]</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>[['G:min', 'D:7', 'G:min'], ['G:min', 'C:min/G', 'G:min']]</t>
+          <t>[['Eb', 'Eb:7', 'Ab']]</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>[(74.1, 80.04), (25.48, 32.58)]</t>
+          <t>[(16.192174, 27.488682)]</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>[(2.58, 5.02), (0.22, 3.44)]</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>spotify:track:2g41AZ58LFdQLxmWx82ujI</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>spotify:track:4lrfYSnZmpXdCWuWqVo8L0</t>
-        </is>
-      </c>
+          <t>[(45.01, 49.44)]</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>isophonics_89</t>
+          <t>jaah_49</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>isophonics_157</t>
+          <t>schubert-winterreise_156</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.1691176470588235</v>
+        <v>0.07061307475758523</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>[['F#', 'B', 'F#']]</t>
+          <t>[['F:7', 'Bb', 'Bb']]</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>[['E', 'A', 'E']]</t>
+          <t>[['C#:7', 'F#:maj', 'F#:maj/A#']]</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>[(15.880484, 21.522933)]</t>
+          <t>[(44.74, 47.14)]</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>[(2.612267, 17.443474)]</t>
+          <t>[(21.44, 24.06)]</t>
         </is>
       </c>
       <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>spotify:track:4lrfYSnZmpXdCWuWqVo8L0</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>isophonics_295</t>
+          <t>isophonics_0</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>isophonics_51</t>
+          <t>jaah_47</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.109375</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>[['F/3', 'G/3', 'C']]</t>
+          <t>[['Db:7', 'Gb', 'Gb']]</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>[['F', 'G', 'C']]</t>
+          <t>[['Db:7', 'Gb', 'Gb']]</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>[(135.871449, 138.80365)]</t>
+          <t>[(28.079297, 32.374988)]</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>[(25.687641, 32.084739)]</t>
+          <t>[(20.14, 23.58)]</t>
         </is>
       </c>
       <c r="H13" t="inlineStr"/>
@@ -959,76 +963,72 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>isophonics_0</t>
+          <t>jaah_65</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>isophonics_283</t>
+          <t>jaah_62</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.03180619644034278</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>[['Db', 'Gb', 'Ab', 'Db']]</t>
+          <t>[['F:7', 'Bb:min7', 'Eb:7']]</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>[['G', 'C', 'D', 'G']]</t>
+          <t>[['D:7', 'G:min7', 'C:7']]</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>[(0.344657, 7.314387)]</t>
+          <t>[(7.42, 9.26)]</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>[(63.629047, 74.101247)]</t>
+          <t>[(29.42, 30.52)]</t>
         </is>
       </c>
       <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>spotify:track:3tGhRLgcCP6SIZU3tbGl7l</t>
-        </is>
-      </c>
+      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>isophonics_12</t>
+          <t>isophonics_149</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>isophonics_81</t>
+          <t>isophonics_288</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.2666666666666667</v>
+        <v>0.2094017094017094</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>[['G', 'A', 'D', 'D']]</t>
+          <t>[['B', 'F#', 'B', 'E'], ['C#', 'F#', 'E', 'B']]</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>[['E', 'F#', 'B', 'B']]</t>
+          <t>[['E', 'B', 'E', 'A'], ['F#', 'B', 'A/9', 'E/5']]</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>[(9.979342, 16.701519)]</t>
+          <t>[(45.875873, 53.747437), (56.394512, 66.994421)]</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>[(52.727278, 61.620521)]</t>
+          <t>[(38.714036, 44.240385), (59.356575, 64.894535)]</t>
         </is>
       </c>
       <c r="H15" t="inlineStr"/>
@@ -1037,84 +1037,84 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>schubert-winterreise_52</t>
+          <t>isophonics_61</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>schubert-winterreise_194</t>
+          <t>schubert-winterreise_14</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.1712473572938689</v>
+        <v>0.162280701754386</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>[['D:min', 'A:7/E', 'D:min']]</t>
+          <t>[['F#:min', 'C#', 'F#:min']]</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>[['C:min', 'G:7/D', 'C:min/D#']]</t>
+          <t>[['D:min', 'A:maj', 'D:min']]</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>[(1.44, 6.66)]</t>
+          <t>[(3.744784, 6.774988)]</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>[(2.0, 4.32)]</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>spotify:track:5UYEp9kllA47IhttiiMuJ0</t>
-        </is>
-      </c>
+          <t>[(10.56, 17.34)]</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>schubert-winterreise_188</t>
+          <t>schubert-winterreise_88</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>isophonics_287</t>
+          <t>schubert-winterreise_55</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.146875</v>
+        <v>0.2657342657342657</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>[['A#:maj', 'F:maj', 'A#:maj'], ['F:maj', 'A#:maj', 'F:maj']]</t>
+          <t>[['A:maj/E', 'E:7', 'A:maj', 'E:7', 'A:maj']]</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>[['D', 'A', 'D'], ['A/3', 'D', 'A']]</t>
+          <t>[['G:maj', 'D:7/C', 'G:maj/B', 'D:7/C', 'G:maj/B']]</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>[(132.38, 134.0), (128.76, 133.56)]</t>
+          <t>[(16.04, 21.0)]</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>[(21.722199, 26.760929), (65.81034, 71.679931)]</t>
+          <t>[(68.64, 83.84)]</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>spotify:track:1nvxQGWCnikMK7a4HYQvSx</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr"/>
+          <t>spotify:track:0XfunCHFEeQnzm4NaY8rJr</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>spotify:track:68YORkKP9uvlOQFMZZZwH5</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updated harmonic similarity files
</commit_message>
<xml_diff>
--- a/hsim-experiment/harmonic_similarity_split/harmonic_similarity_matches_1.xlsx
+++ b/hsim-experiment/harmonic_similarity_split/harmonic_similarity_matches_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,45 +436,50 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>similarity_range</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>track_1</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>track_2</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>sim_val</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>pattern_track_1</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>pattern_track_2</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>time_pattern_track_1</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>time_pattern_track_2</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>link_track_1</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>link_track_2</t>
         </is>
@@ -483,88 +488,90 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>schubert-winterreise_61</t>
+          <t>low</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>schubert-winterreise_89</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>0.1177257525083612</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>[['C:min/D#', 'G:min/D', 'D:7', 'G:min']]</t>
-        </is>
+          <t>schubert-winterreise_211</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>schubert-winterreise_109</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.2003577817531306</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[['C:min/G', 'G:min', 'D:7', 'G:min']]</t>
+          <t>[['C:7/E', 'F:maj', 'C:7/E', 'F:maj']]</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[(42.14, 44.36)]</t>
+          <t>[['C:7', 'F:maj/C', 'C:7', 'F:maj']]</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[(2.98, 6.7)]</t>
+          <t>[('0:00:36.500000', '0:00:41.660000')]</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>spotify:track:68YORkKP9uvlOQFMZZZwH5</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>spotify:track:4lrfYSnZmpXdCWuWqVo8L0</t>
+          <t>[('0:01:37.640000', '0:01:51')]</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>spotify:track:5UYEp9kllA47IhttiiMuJ0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>schubert-winterreise_164</t>
+          <t>low</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>schubert-winterreise_157</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>0.2753623188405797</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>[['A:min', 'D:min', 'A:min', 'E:7', 'A:min']]</t>
-        </is>
+          <t>isophonics_196</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>schubert-winterreise_9</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.09351927809680066</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[['F:min', 'A#:min/F', 'F:min', 'C:7', 'F:min']]</t>
+          <t>[['D/5', 'A', 'D/5']]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>[(14.52, 29.1)]</t>
+          <t>[['F:maj', 'C:maj', 'F:maj']]</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>[(0.3, 4.8)]</t>
+          <t>[('0:00:31.898979', '0:00:34.035215')]</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>spotify:track:3OD2uwEUQKg0WyW9Lewata</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
+          <t>[('0:00:46.600000', '0:00:49.040000')]</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
         <is>
           <t>spotify:track:4lrfYSnZmpXdCWuWqVo8L0</t>
         </is>
@@ -573,548 +580,580 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>isophonics_30</t>
+          <t>low</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>isophonics_107</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>0.1894736842105263</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>[['A', 'A', 'D']]</t>
-        </is>
+          <t>jaah_7</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>jaah_45</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.01724644781969623</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[['E', 'E', 'A']]</t>
+          <t>[['F:7', 'Bb:7', 'Eb:maj6']]</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>[(14.448702, 17.908476)]</t>
+          <t>[['F:7', 'Bb:7', 'Eb:maj6']]</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>[(122.976598, 130.383764)]</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr"/>
+          <t>[('0:00:14.240000', '0:00:17.770000')]</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>[('0:00:38.760000', '0:00:41.580000')]</t>
+        </is>
+      </c>
       <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>isophonics_297</t>
+          <t>low</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>isophonics_199</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>0.06725146198830409</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>[['C', 'D', 'G']]</t>
-        </is>
+          <t>isophonics_61</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>isophonics_238</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.112280701754386</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[['G', 'A', 'D']]</t>
+          <t>[['C#', 'F#:min', 'F#:min']]</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>[(18.675377, 23.261318)]</t>
+          <t>[['C', 'F:min', 'F:min/5']]</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>[(2.088054, 5.756807)]</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr"/>
+          <t>[('0:01:00.865873', '0:01:03.512947')]</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>[('0:00:41.384331', '0:00:46.388231')]</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>spotify:track:5By7Pzgl6TMuVJG168VWzS</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>schubert-winterreise_69</t>
+          <t>low</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>schubert-winterreise_6</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>0.1384615384615385</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>[['B:min', 'F#:7/A#', 'B:min']]</t>
-        </is>
+          <t>jaah_0</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>schubert-winterreise_66</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.07672413793103448</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>[['B:min/F#', 'F#:7', 'B:min']]</t>
+          <t>[['Ab', 'Eb:7', 'Ab']]</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>[(42.36, 50.36)]</t>
+          <t>[['C/G', 'G:7', 'C']]</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>[(79.42, 86.02)]</t>
+          <t>[('0:00:25.220000', '0:00:27.170000')]</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>spotify:track:1yerCi2iQCVkdHG6rdRn7R</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>spotify:track:2g41AZ58LFdQLxmWx82ujI</t>
-        </is>
-      </c>
+          <t>[('0:04:22.920000', '0:04:26.900000')]</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>isophonics_93</t>
+          <t>mid</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>isophonics_261</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>0.1154891304347826</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>[['C', 'F:maj6', 'C']]</t>
-        </is>
+          <t>schubert-winterreise_163</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>schubert-winterreise_196</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.5333333333333333</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>[['G', 'A:min7', 'G/3']]</t>
+          <t>[['C:7', 'F:maj', 'C:7', 'F:maj', 'C:7', 'F:maj']]</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>[(36.36882, 43.729546)]</t>
+          <t>[['D:7', 'G:maj', 'D:7', 'G:maj', 'D:7', 'G:maj']]</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>[(10.107052, 14.565283)]</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr"/>
+          <t>[('0:01:47.900000', '0:01:49.300000')]</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>[('0:00:35.460000', '0:00:50.440000')]</t>
+        </is>
+      </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>spotify:track:2B4Y9u4ERAFiMo13XPJyGP</t>
-        </is>
-      </c>
+          <t>spotify:track:1nvxQGWCnikMK7a4HYQvSx</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>isophonics_31</t>
+          <t>hi</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>isophonics_251</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>0.3101503759398496</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>[['E:min', 'C', 'G', 'C', 'G']]</t>
-        </is>
+          <t>schubert-winterreise_169</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>schubert-winterreise_137</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>[['B:min', 'G', 'D', 'G', 'D']]</t>
+          <t>[['G:min', 'C:min', 'G:min', 'D:7', 'G:min', 'A#:maj/D', 'D#:maj', 'F:7', 'A#:maj', 'G:min/D', 'D:7', 'G:min', 'G:min/D', 'D:7', 'G:min']]</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>[(11.110106, 30.271443)]</t>
+          <t>[['A:min', 'D:min', 'A:min', 'E:7', 'A:min', 'C:maj/E', 'F:maj', 'G:7', 'C:maj', 'A:min/E', 'E:7', 'A:min', 'A:min/E', 'E:7', 'A:min']]</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>[(22.141972, 33.3456)]</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
+          <t>[('0:00:14.520000', '0:00:59.040000')]</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>[('0:00:14.900000', '0:00:56.280000')]</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>spotify:track:3OD2uwEUQKg0WyW9Lewata</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>spotify:track:3OD2uwEUQKg0WyW9Lewata</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>isophonics_111</t>
+          <t>mid</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>schubert-winterreise_63</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>0.1613636363636363</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>[['C', 'G:7', 'C']]</t>
-        </is>
+          <t>isophonics_58</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>isophonics_52</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.4017857142857143</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>[['C/G', 'G:7', 'C']]</t>
+          <t>[['C', 'C:7', 'F', 'C', 'G']]</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>[(70.519024, 75.720294)]</t>
+          <t>[['G', 'G:7', 'C', 'G', 'D']]</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>[(253.84, 257.6)]</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr"/>
+          <t>[('0:00:31.527551', '0:00:54.712675')]</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>[('0:00:58.265237', '0:01:10.536984')]</t>
+        </is>
+      </c>
       <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>schubert-winterreise_188</t>
+          <t>mid</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>isophonics_212</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>[['F:maj', 'A#:maj', 'F:maj', 'A#:maj', 'F:maj']]</t>
-        </is>
+          <t>schubert-winterreise_147</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>schubert-winterreise_31</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.5050505050505051</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>[['D', 'G', 'D', 'G', 'D']]</t>
+          <t>[['A:maj/E', 'E:7', 'A:maj', 'E:7', 'A:maj']]</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>[(128.76, 134.6)]</t>
+          <t>[['G:maj', 'D:7', 'G:maj', 'D:7', 'G:maj']]</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>[(46.93228, 57.636679)]</t>
+          <t>[('0:00:19.780000', '0:00:25.820000')]</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>spotify:track:1nvxQGWCnikMK7a4HYQvSx</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr"/>
+          <t>[('0:00:07.900000', '0:00:20.520000')]</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>spotify:track:0XfunCHFEeQnzm4NaY8rJr</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>isophonics_213</t>
+          <t>mid</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>jaah_43</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>0.1607142857142857</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>[['E', 'E:7', 'A']]</t>
-        </is>
+          <t>schubert-winterreise_2</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>schubert-winterreise_117</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.5050505050505051</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>[['Eb', 'Eb:7', 'Ab']]</t>
+          <t>[['A:maj/E', 'E:7', 'A:maj', 'E:7', 'A:maj']]</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>[(16.192174, 27.488682)]</t>
+          <t>[['G:maj', 'D:7', 'G:maj', 'D:7', 'G:maj']]</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>[(45.01, 49.44)]</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
+          <t>[('0:00:20.560000', '0:00:26.400000')]</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>[('0:00:07.160000', '0:00:19.200000')]</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>spotify:track:0XfunCHFEeQnzm4NaY8rJr</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>jaah_49</t>
+          <t>mid</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>schubert-winterreise_156</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>0.07061307475758523</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>[['F:7', 'Bb', 'Bb']]</t>
-        </is>
+          <t>schubert-winterreise_182</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>schubert-winterreise_153</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.5142857142857142</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>[['C#:7', 'F#:maj', 'F#:maj/A#']]</t>
+          <t>[['D:maj/A', 'G:maj', 'D:maj/A']]</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>[(44.74, 47.14)]</t>
+          <t>[['G:maj/B', 'C:maj', 'G:maj/D']]</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>[(21.44, 24.06)]</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>spotify:track:4lrfYSnZmpXdCWuWqVo8L0</t>
-        </is>
-      </c>
+          <t>[('0:02:34.020000', '0:02:39.240000')]</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>[('0:00:58.400000', '0:01:00.680000')]</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>isophonics_0</t>
+          <t>hi</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>jaah_47</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>0.109375</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>[['Db:7', 'Gb', 'Gb']]</t>
-        </is>
+          <t>schubert-winterreise_1</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>schubert-winterreise_102</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>[['Db:7', 'Gb', 'Gb']]</t>
+          <t>[['E:7', 'A:maj', 'A:maj', 'E:7/G#', 'C#:7', 'F#:min', 'A:maj/E', 'E:7', 'A:maj', 'E:7', 'A:maj']]</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>[(28.079297, 32.374988)]</t>
+          <t>[['D:7', 'G:maj', 'G:maj', 'D:7/F#', 'B:7', 'E:min', 'G:maj/D', 'D:7', 'G:maj', 'D:7', 'G:maj']]</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>[(20.14, 23.58)]</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
+          <t>[('0:00:07.020000', '0:00:24.780000')]</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>[('0:00:06.740000', '0:00:21.540000')]</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>spotify:track:0XfunCHFEeQnzm4NaY8rJr</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>spotify:track:0XfunCHFEeQnzm4NaY8rJr</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>jaah_65</t>
+          <t>hi</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>jaah_62</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>0.03180619644034278</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>[['F:7', 'Bb:min7', 'Eb:7']]</t>
-        </is>
+          <t>schubert-winterreise_4</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>schubert-winterreise_78</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>[['D:7', 'G:min7', 'C:7']]</t>
+          <t>[['A:maj', 'D:maj', 'E:9/G#', 'A:maj', 'B:7/F#', 'E:min', 'A:(3,5,b7,b9)', 'D:maj', 'G:maj', 'D:maj/F#', 'A:min/E', 'B:maj/D#', 'C:maj/E', 'D:7/F#', 'G:maj', 'E:min7/G', 'E:(3,5,b7,b9)/G#', 'A:maj']]</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>[(7.42, 9.26)]</t>
+          <t>[['A:maj', 'D:maj', 'E:9/G#', 'A:maj', 'B:7/F#', 'E:min', 'A:(3,5,b7,b9)', 'D:maj', 'G:maj', 'D:maj/F#', 'A:min/E', 'B:maj/D#', 'C:maj/E', 'D:7/F#', 'G:maj', 'E:min7/G', 'E:(3,5,b7,b9)/G#', 'A:maj']]</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>[(29.42, 30.52)]</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr"/>
+          <t>[('0:00:58.080000', '0:01:19.120000')]</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>[('0:00:53.120000', '0:01:14.300000')]</t>
+        </is>
+      </c>
       <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>isophonics_149</t>
+          <t>hi</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>isophonics_288</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>0.2094017094017094</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>[['B', 'F#', 'B', 'E'], ['C#', 'F#', 'E', 'B']]</t>
-        </is>
+          <t>schubert-winterreise_24</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>schubert-winterreise_125</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>[['E', 'B', 'E', 'A'], ['F#', 'B', 'A/9', 'E/5']]</t>
+          <t>[['E:(3,b5,b7)/G#', 'A:maj', 'E:(3,b5,b7)/A#', 'A:maj', 'E:(3,b5,b7)/A#', 'A:maj', 'E:(3,b5,b7)/A#', 'A:maj', 'E:(3,b5,b7)/A#', 'A:maj', 'E:(3,b5,b7)/A#']]</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>[(45.875873, 53.747437), (56.394512, 66.994421)]</t>
+          <t>[['E:(3,b5,b7)/G#', 'A:maj', 'E:(3,b5,b7)/A#', 'A:maj', 'E:(3,b5,b7)/A#', 'A:maj', 'E:(3,b5,b7)/A#', 'A:maj', 'E:(3,b5,b7)/A#', 'A:maj', 'E:(3,b5,b7)/A#']]</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>[(38.714036, 44.240385), (59.356575, 64.894535)]</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr"/>
+          <t>[('0:00:51.700000', '0:00:57.700000')]</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>[('0:00:48.440000', '0:00:53.480000')]</t>
+        </is>
+      </c>
       <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>isophonics_61</t>
+          <t>hi</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>schubert-winterreise_14</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>0.162280701754386</v>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>[['F#:min', 'C#', 'F#:min']]</t>
-        </is>
+          <t>schubert-winterreise_90</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>schubert-winterreise_17</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>[['D:min', 'A:maj', 'D:min']]</t>
+          <t>[['G:maj', 'E:7/G#', 'A:min', 'D:7/F#', 'G:maj']]</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>[(3.744784, 6.774988)]</t>
+          <t>[['G:maj', 'E:7/G#', 'A:min', 'D:7/F#', 'G:maj']]</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>[(10.56, 17.34)]</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr"/>
+          <t>[('0:01:20.920000', '0:01:29.040000')]</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>[('0:01:12.080000', '0:01:19.580000')]</t>
+        </is>
+      </c>
       <c r="I16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>schubert-winterreise_88</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>schubert-winterreise_55</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>0.2657342657342657</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>[['A:maj/E', 'E:7', 'A:maj', 'E:7', 'A:maj']]</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>[['G:maj', 'D:7/C', 'G:maj/B', 'D:7/C', 'G:maj/B']]</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>[(16.04, 21.0)]</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>[(68.64, 83.84)]</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>spotify:track:0XfunCHFEeQnzm4NaY8rJr</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>spotify:track:68YORkKP9uvlOQFMZZZwH5</t>
-        </is>
-      </c>
+      <c r="J16" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>